<commit_message>
Script zusammenfassung bis 2.3.3
</commit_message>
<xml_diff>
--- a/NullNUMMER24/M159-Teil1_AB02---gelöst.xlsx
+++ b/NullNUMMER24/M159-Teil1_AB02---gelöst.xlsx
@@ -352,7 +352,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -397,12 +397,6 @@
       <name val="Verdana"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -588,276 +582,264 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="65">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="9" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="9" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -944,9 +926,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>1850760</xdr:colOff>
+      <xdr:colOff>1850400</xdr:colOff>
       <xdr:row>74</xdr:row>
-      <xdr:rowOff>101160</xdr:rowOff>
+      <xdr:rowOff>100800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -959,8 +941,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7666200" y="8883000"/>
-          <a:ext cx="7925400" cy="5216040"/>
+          <a:off x="7665480" y="8883000"/>
+          <a:ext cx="7925040" cy="5215680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -982,90 +964,90 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C45" activeCellId="0" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="41.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="45.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="260.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="38.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="41.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="45.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="260.95"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="1" t="s">
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="4" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="6" t="s">
+      <c r="G2" s="6"/>
+      <c r="H2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="3"/>
+      <c r="I2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="9" t="s">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="11"/>
-      <c r="I3" s="7"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="8"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12" t="n">
+      <c r="A4" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="13" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="13"/>
       <c r="E4" s="14"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="11"/>
       <c r="H4" s="15"/>
-      <c r="I4" s="12" t="s">
+      <c r="I4" s="13" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1286,7 +1268,7 @@
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="25"/>
       <c r="B19" s="25"/>
-      <c r="C19" s="46" t="s">
+      <c r="C19" s="45" t="s">
         <v>35</v>
       </c>
       <c r="D19" s="28"/>
@@ -1299,7 +1281,7 @@
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="25"/>
       <c r="B20" s="25"/>
-      <c r="C20" s="46" t="s">
+      <c r="C20" s="45" t="s">
         <v>36</v>
       </c>
       <c r="D20" s="28"/>
@@ -1312,7 +1294,7 @@
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="25"/>
       <c r="B21" s="25"/>
-      <c r="C21" s="47" t="s">
+      <c r="C21" s="46" t="s">
         <v>37</v>
       </c>
       <c r="D21" s="41"/>
@@ -1326,7 +1308,7 @@
       <c r="A22" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="B22" s="48" t="s">
+      <c r="B22" s="17" t="s">
         <v>38</v>
       </c>
       <c r="C22" s="42" t="s">
@@ -1352,7 +1334,7 @@
       <c r="B23" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="C23" s="49" t="s">
+      <c r="C23" s="47" t="s">
         <v>43</v>
       </c>
       <c r="D23" s="28"/>
@@ -1406,7 +1388,7 @@
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="25"/>
       <c r="B27" s="39"/>
-      <c r="C27" s="50"/>
+      <c r="C27" s="48"/>
       <c r="D27" s="35"/>
       <c r="E27" s="36"/>
       <c r="F27" s="30"/>
@@ -1417,7 +1399,7 @@
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="25"/>
       <c r="B28" s="39"/>
-      <c r="C28" s="51" t="s">
+      <c r="C28" s="49" t="s">
         <v>48</v>
       </c>
       <c r="D28" s="38" t="s">
@@ -1436,7 +1418,7 @@
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="25"/>
       <c r="B29" s="39"/>
-      <c r="C29" s="52" t="s">
+      <c r="C29" s="50" t="s">
         <v>46</v>
       </c>
       <c r="D29" s="28"/>
@@ -1449,7 +1431,7 @@
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="25"/>
       <c r="B30" s="39"/>
-      <c r="C30" s="53" t="s">
+      <c r="C30" s="51" t="s">
         <v>50</v>
       </c>
       <c r="D30" s="41"/>
@@ -1462,7 +1444,7 @@
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="25"/>
       <c r="B31" s="39"/>
-      <c r="C31" s="53" t="s">
+      <c r="C31" s="51" t="s">
         <v>47</v>
       </c>
       <c r="D31" s="41"/>
@@ -1476,13 +1458,13 @@
       <c r="A32" s="16" t="n">
         <v>5</v>
       </c>
-      <c r="B32" s="48" t="s">
+      <c r="B32" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="C32" s="54" t="s">
+      <c r="C32" s="52" t="s">
         <v>52</v>
       </c>
-      <c r="D32" s="55" t="s">
+      <c r="D32" s="53" t="s">
         <v>53</v>
       </c>
       <c r="E32" s="20" t="s">
@@ -1530,7 +1512,7 @@
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="25"/>
       <c r="B35" s="39"/>
-      <c r="C35" s="46"/>
+      <c r="C35" s="45"/>
       <c r="D35" s="28"/>
       <c r="E35" s="36"/>
       <c r="F35" s="30"/>
@@ -1541,10 +1523,10 @@
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="25"/>
       <c r="B36" s="39"/>
-      <c r="C36" s="56" t="s">
+      <c r="C36" s="54" t="s">
         <v>48</v>
       </c>
-      <c r="D36" s="57" t="s">
+      <c r="D36" s="55" t="s">
         <v>49</v>
       </c>
       <c r="E36" s="29"/>
@@ -1560,7 +1542,7 @@
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="25"/>
       <c r="B37" s="39"/>
-      <c r="C37" s="52" t="s">
+      <c r="C37" s="50" t="s">
         <v>56</v>
       </c>
       <c r="D37" s="28"/>
@@ -1573,7 +1555,7 @@
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="25"/>
       <c r="B38" s="39"/>
-      <c r="C38" s="52" t="s">
+      <c r="C38" s="50" t="s">
         <v>50</v>
       </c>
       <c r="D38" s="28"/>
@@ -1586,7 +1568,7 @@
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="25"/>
       <c r="B39" s="39"/>
-      <c r="C39" s="56" t="s">
+      <c r="C39" s="54" t="s">
         <v>47</v>
       </c>
       <c r="D39" s="28"/>
@@ -1597,15 +1579,15 @@
       <c r="I39" s="33"/>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="58"/>
-      <c r="B40" s="59"/>
-      <c r="C40" s="60"/>
+      <c r="A40" s="56"/>
+      <c r="B40" s="40"/>
+      <c r="C40" s="57"/>
       <c r="D40" s="41"/>
-      <c r="E40" s="61"/>
-      <c r="F40" s="62"/>
-      <c r="G40" s="63"/>
-      <c r="H40" s="64"/>
-      <c r="I40" s="65"/>
+      <c r="E40" s="58"/>
+      <c r="F40" s="59"/>
+      <c r="G40" s="60"/>
+      <c r="H40" s="61"/>
+      <c r="I40" s="62"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="25" t="n">
@@ -1614,10 +1596,10 @@
       <c r="B41" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="C41" s="54" t="s">
+      <c r="C41" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="D41" s="55" t="s">
+      <c r="D41" s="53" t="s">
         <v>53</v>
       </c>
       <c r="E41" s="29" t="s">
@@ -1639,7 +1621,7 @@
       <c r="B42" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="C42" s="46"/>
+      <c r="C42" s="45"/>
       <c r="D42" s="28"/>
       <c r="E42" s="36"/>
       <c r="F42" s="30"/>
@@ -1650,7 +1632,7 @@
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="25"/>
       <c r="B43" s="39"/>
-      <c r="C43" s="46"/>
+      <c r="C43" s="45"/>
       <c r="D43" s="28"/>
       <c r="E43" s="36"/>
       <c r="F43" s="30"/>
@@ -1661,7 +1643,7 @@
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="25"/>
       <c r="B44" s="39"/>
-      <c r="C44" s="46"/>
+      <c r="C44" s="45"/>
       <c r="D44" s="28"/>
       <c r="E44" s="36"/>
       <c r="F44" s="30"/>
@@ -1672,7 +1654,7 @@
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="25"/>
       <c r="B45" s="39"/>
-      <c r="C45" s="46"/>
+      <c r="C45" s="45"/>
       <c r="D45" s="28"/>
       <c r="E45" s="36"/>
       <c r="F45" s="30"/>
@@ -1683,7 +1665,7 @@
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="25"/>
       <c r="B46" s="39"/>
-      <c r="C46" s="46"/>
+      <c r="C46" s="45"/>
       <c r="D46" s="28"/>
       <c r="E46" s="36"/>
       <c r="F46" s="30"/>
@@ -1692,58 +1674,58 @@
       <c r="I46" s="33"/>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="58"/>
-      <c r="B47" s="59"/>
-      <c r="C47" s="47"/>
+      <c r="A47" s="56"/>
+      <c r="B47" s="40"/>
+      <c r="C47" s="46"/>
       <c r="D47" s="41"/>
-      <c r="E47" s="61"/>
-      <c r="F47" s="62"/>
-      <c r="G47" s="63"/>
-      <c r="H47" s="64"/>
-      <c r="I47" s="65"/>
+      <c r="E47" s="58"/>
+      <c r="F47" s="59"/>
+      <c r="G47" s="60"/>
+      <c r="H47" s="61"/>
+      <c r="I47" s="62"/>
     </row>
     <row r="50" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="66" t="s">
+      <c r="B50" s="63" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="67" t="s">
+      <c r="B51" s="64" t="s">
         <v>61</v>
       </c>
-      <c r="C51" s="0" t="s">
+      <c r="C51" s="1" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="67" t="s">
+      <c r="B52" s="64" t="s">
         <v>63</v>
       </c>
-      <c r="C52" s="0" t="s">
+      <c r="C52" s="1" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="67" t="s">
+      <c r="B53" s="64" t="s">
         <v>65</v>
       </c>
-      <c r="C53" s="0" t="s">
+      <c r="C53" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B54" s="67" t="s">
+      <c r="B54" s="64" t="s">
         <v>67</v>
       </c>
-      <c r="C54" s="0" t="s">
+      <c r="C54" s="1" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="67" t="s">
+      <c r="B55" s="64" t="s">
         <v>69</v>
       </c>
-      <c r="C55" s="0" t="s">
+      <c r="C55" s="1" t="s">
         <v>70</v>
       </c>
     </row>

</xml_diff>